<commit_message>
Added assembly instructions and updated readme
</commit_message>
<xml_diff>
--- a/Hardware/KiCad/plots/Mouse_BOM.xlsx
+++ b/Hardware/KiCad/plots/Mouse_BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="131">
   <si>
     <t xml:space="preserve">MOUSE BOM</t>
   </si>
@@ -124,6 +124,15 @@
     <t xml:space="preserve">LED_D5.0mm_Horizontal_O1.27mm_Z3.0mm</t>
   </si>
   <si>
+    <t xml:space="preserve">RED LED 630nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C503B-RAN-CZ0C0AA1</t>
+  </si>
+  <si>
     <t xml:space="preserve">DNP</t>
   </si>
   <si>
@@ -334,6 +343,12 @@
     <t xml:space="preserve">ADNS2610</t>
   </si>
   <si>
+    <t xml:space="preserve">Optical Sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avago</t>
+  </si>
+  <si>
     <t xml:space="preserve">ADNS2610PTH</t>
   </si>
   <si>
@@ -346,6 +361,15 @@
     <t xml:space="preserve">ENCODER-QUADRATURE</t>
   </si>
   <si>
+    <t xml:space="preserve">Cloukeu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mouse Encoder 9mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.aliexpress.com/item/10Pcs-5MM-7MM-9MM-11MM-13MM-Mouse-encoder-11mm-wheel-decoder/32457386770.html?spm=a2g0s.9042311.0.0.40924c4d4qPTtC</t>
+  </si>
+  <si>
     <t xml:space="preserve">U3</t>
   </si>
   <si>
@@ -368,6 +392,12 @@
   </si>
   <si>
     <t xml:space="preserve">24MHz Resonator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TDK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FCR24.0M6T</t>
   </si>
   <si>
     <t xml:space="preserve">Y2</t>
@@ -496,7 +526,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,12 +575,6 @@
         <bgColor rgb="FFFFCCCC"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF7F00"/>
-        <bgColor rgb="FFFF9900"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
@@ -669,7 +693,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -745,7 +769,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF7F00"/>
+      <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -766,10 +790,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -989,13 +1013,13 @@
         <v>34</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1004,7 +1028,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>10</v>
@@ -1013,13 +1037,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H10" s="1"/>
     </row>
@@ -1029,7 +1053,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>10</v>
@@ -1038,13 +1062,13 @@
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -1054,22 +1078,22 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -1079,22 +1103,22 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -1104,25 +1128,25 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D14" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1131,25 +1155,25 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D15" s="3" t="n">
         <v>2</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1158,22 +1182,22 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -1183,22 +1207,22 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -1208,7 +1232,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>10</v>
@@ -1217,13 +1241,13 @@
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -1233,7 +1257,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>10</v>
@@ -1242,13 +1266,13 @@
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -1258,7 +1282,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>10</v>
@@ -1267,13 +1291,13 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H20" s="1"/>
     </row>
@@ -1283,7 +1307,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>10</v>
@@ -1292,13 +1316,13 @@
         <v>2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H21" s="1"/>
     </row>
@@ -1308,7 +1332,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>10</v>
@@ -1317,13 +1341,13 @@
         <v>3</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H22" s="2"/>
     </row>
@@ -1333,22 +1357,22 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H23" s="1"/>
     </row>
@@ -1358,25 +1382,25 @@
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D24" s="3" t="n">
         <v>2</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,22 +1409,22 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H25" s="1"/>
     </row>
@@ -1410,25 +1434,25 @@
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D26" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>104</v>
+      <c r="E26" s="0" t="s">
+        <v>107</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>34</v>
+        <v>108</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>34</v>
+        <v>109</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1437,25 +1461,28 @@
         <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D27" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>34</v>
+        <v>113</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>34</v>
+        <v>114</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1464,22 +1491,22 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="H28" s="1"/>
     </row>
@@ -1489,25 +1516,25 @@
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="D29" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>34</v>
+        <v>125</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,22 +1543,22 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="H30" s="1"/>
     </row>

</xml_diff>